<commit_message>
s2ganalytics( ) is throwing Google.Apis assembly ref err
</commit_message>
<xml_diff>
--- a/xls/ganalytics_sessions1.xlsx
+++ b/xls/ganalytics_sessions1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-5160" yWindow="900" windowWidth="20115" windowHeight="8010" activeTab="2"/>
@@ -11,12 +11,12 @@
     <sheet name="data" sheetId="3" r:id="rId2"/>
     <sheet name="s2cfg" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>query</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>end_date</t>
-  </si>
-  <si>
-    <t>metricQuery1</t>
   </si>
   <si>
     <t>value</t>
@@ -66,11 +63,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,19 +117,17 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.64bca4930cfe496cabb4ecd3ff574aa5">
+    <main first="rtdsrv.eefbb98aaf7f4352938c098cc5f51220">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
-        <stp>baremetrics.metricQuery1.status</stp>
+        <stp>ganalytics.sessionsQuery1.status</stp>
         <tr r="B3" s="1"/>
       </tp>
-    </main>
-    <main first="rtdsrv.64bca4930cfe496cabb4ecd3ff574aa5">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
-        <stp>baremetrics.metricQuery1.count</stp>
+        <stp>ganalytics.sessionsQuery1.count</stp>
         <tr r="B2" s="1"/>
       </tp>
     </main>
@@ -215,6 +210,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -249,6 +245,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,44 +421,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="str">
-        <f>_xll.s2baremetrics(A1)</f>
-        <v>OK</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <f>_xll.s2ganalytics(A1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="e">
-        <f ca="1">_xll.s2sub(s2cfg!$A$1,$A$1,A2)</f>
+        <f>_xll.s2sub(s2cfg!$A$1,$A$1,A2)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="e">
-        <f ca="1">_xll.s2sub(s2cfg!$A$1,$A$1,A3)</f>
+        <f>_xll.s2sub(s2cfg!$A$1,$A$1,A3)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -471,15 +468,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -496,185 +493,185 @@
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="str">
         <f>_xll.s2today(-7)</f>
-        <v>2017-04-19</v>
+        <v>2017-04-20</v>
       </c>
       <c r="C1" s="2" t="str">
         <f>_xll.s2today(-6)</f>
-        <v>2017-04-20</v>
+        <v>2017-04-21</v>
       </c>
       <c r="D1" s="2" t="str">
         <f>_xll.s2today(-5)</f>
-        <v>2017-04-21</v>
+        <v>2017-04-22</v>
       </c>
       <c r="E1" s="2" t="str">
         <f>_xll.s2today(-4)</f>
-        <v>2017-04-22</v>
+        <v>2017-04-23</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>_xll.s2today(-3)</f>
-        <v>2017-04-23</v>
+        <v>2017-04-24</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>_xll.s2today(-2)</f>
-        <v>2017-04-24</v>
+        <v>2017-04-25</v>
       </c>
       <c r="H1" s="2" t="str">
         <f>_xll.s2today(-1)</f>
-        <v>2017-04-25</v>
+        <v>2017-04-26</v>
       </c>
       <c r="I1" s="2" t="str">
         <f>_xll.s2today(0)</f>
-        <v>2017-04-26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>2017-04-27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A2)</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <f ca="1">_xll.s2bcache( subs!$A$1,B$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f ca="1">_xll.s2bcache( subs!$A$1,C$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <f ca="1">_xll.s2bcache( subs!$A$1,D$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f ca="1">_xll.s2bcache( subs!$A$1,E$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <f ca="1">_xll.s2bcache( subs!$A$1,F$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <f ca="1">_xll.s2bcache( subs!$A$1,G$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <f ca="1">_xll.s2bcache( subs!$A$1,H$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <f ca="1">_xll.s2bcache( subs!$A$1,I$1,$A2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+      <c r="B3">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A3)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <f ca="1">_xll.s2bcache( subs!$A$1,B$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <f ca="1">_xll.s2bcache( subs!$A$1,C$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <f ca="1">_xll.s2bcache( subs!$A$1,D$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f ca="1">_xll.s2bcache( subs!$A$1,E$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <f ca="1">_xll.s2bcache( subs!$A$1,F$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <f ca="1">_xll.s2bcache( subs!$A$1,G$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f ca="1">_xll.s2bcache( subs!$A$1,H$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f ca="1">_xll.s2bcache( subs!$A$1,I$1,$A3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="B4">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A4)</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
-        <f ca="1">_xll.s2bcache( subs!$A$1,B$1,$A4)</f>
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <f ca="1">_xll.s2bcache( subs!$A$1,C$1,$A4)</f>
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <f ca="1">_xll.s2bcache( subs!$A$1,D$1,$A4)</f>
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f ca="1">_xll.s2bcache( subs!$A$1,E$1,$A4)</f>
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <f ca="1">_xll.s2bcache( subs!$A$1,F$1,$A4)</f>
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <f ca="1">_xll.s2bcache( subs!$A$1,G$1,$A4)</f>
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <f ca="1">_xll.s2bcache( subs!$A$1,H$1,$A4)</f>
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <f ca="1">_xll.s2bcache( subs!$A$1,I$1,$A4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
       <c r="B5">
-        <f ca="1">_xll.s2bcache( subs!$A$1,B$1,$A5)</f>
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A5)</f>
         <v>0</v>
       </c>
       <c r="C5">
-        <f ca="1">_xll.s2bcache( subs!$A$1,C$1,$A5)</f>
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A5)</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f ca="1">_xll.s2bcache( subs!$A$1,D$1,$A5)</f>
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A5)</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f ca="1">_xll.s2bcache( subs!$A$1,E$1,$A5)</f>
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A5)</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f ca="1">_xll.s2bcache( subs!$A$1,F$1,$A5)</f>
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A5)</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f ca="1">_xll.s2bcache( subs!$A$1,G$1,$A5)</f>
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A5)</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f ca="1">_xll.s2bcache( subs!$A$1,H$1,$A5)</f>
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A5)</f>
         <v>0</v>
       </c>
       <c r="I5">
-        <f ca="1">_xll.s2bcache( subs!$A$1,I$1,$A5)</f>
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A5)</f>
         <v>0</v>
       </c>
     </row>
@@ -684,15 +681,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -704,38 +701,38 @@
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="str">
         <f>_xll.s2today(-7)</f>
-        <v>2017-04-19</v>
+        <v>2017-04-20</v>
       </c>
       <c r="J1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="str">
         <f>_xll.s2today( 0)</f>
-        <v>2017-04-26</v>
+        <v>2017-04-27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>